<commit_message>
Feature: import csv file
</commit_message>
<xml_diff>
--- a/Import_Excel_Files/PositionMasterData.xlsx
+++ b/Import_Excel_Files/PositionMasterData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hengky_Sanjaya\#_Kuliah\Sems_3\Database Systems\FinalProjectDB\Import_Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0007ACB8-70E0-4F8F-9B2C-A34E5DF094AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02C0177-0C3B-456C-9443-ACE5398B11F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3F38F6C1-67F8-4A91-9BC0-FC37D0D00734}"/>
   </bookViews>
@@ -721,7 +721,7 @@
   <dimension ref="A1:A109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>